<commit_message>
Added Pitot Flow Chart for reference
</commit_message>
<xml_diff>
--- a/quick_look.xlsx
+++ b/quick_look.xlsx
@@ -62,11 +62,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -258,7 +259,7 @@
     <xf numFmtId="164" fontId="11" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="164" fontId="4" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -276,6 +277,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -371,14 +376,14 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <c:chart>
     <c:plotArea>
       <c:scatterChart>
-        <c:scatterStyle val="line"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -406,7 +411,13 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -528,7 +539,13 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+            </c:spPr>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -650,7 +667,13 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+            </c:spPr>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -746,11 +769,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="83035156"/>
-        <c:axId val="20734491"/>
+        <c:axId val="13478453"/>
+        <c:axId val="12282247"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83035156"/>
+        <c:axId val="13478453"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.9"/>
@@ -796,13 +819,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20734491"/>
+        <c:crossAx val="12282247"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="0.005"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="20734491"/>
+        <c:axId val="12282247"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.2"/>
@@ -818,7 +841,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -847,7 +870,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83035156"/>
+        <c:crossAx val="13478453"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -888,16 +911,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>314280</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>37800</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>531000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>494640</xdr:colOff>
-      <xdr:row>90</xdr:row>
-      <xdr:rowOff>150840</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>711360</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>113400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -905,7 +928,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7413480" y="200160"/>
+        <a:off x="6817320" y="0"/>
         <a:ext cx="5869800" cy="14581080"/>
       </xdr:xfrm>
       <a:graphic>
@@ -926,8 +949,8 @@
   </sheetPr>
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G30" activeCellId="0" sqref="G30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G37" activeCellId="0" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1024,7 +1047,7 @@
         <f aca="false">B8+$F$6</f>
         <v>558.863244433801</v>
       </c>
-      <c r="G8" s="4" t="n">
+      <c r="G8" s="5" t="n">
         <f aca="false">(F8/B8)*C8</f>
         <v>0.431147168419821</v>
       </c>
@@ -1052,7 +1075,7 @@
         <f aca="false">B9+$F$6</f>
         <v>564.599034989224</v>
       </c>
-      <c r="G9" s="4" t="n">
+      <c r="G9" s="5" t="n">
         <f aca="false">(F9/B9)*C9</f>
         <v>0.432625212966329</v>
       </c>
@@ -1080,7 +1103,7 @@
         <f aca="false">B10+$F$6</f>
         <v>570.334825544647</v>
       </c>
-      <c r="G10" s="4" t="n">
+      <c r="G10" s="5" t="n">
         <f aca="false">(F10/B10)*C10</f>
         <v>0.432903373641659</v>
       </c>
@@ -1108,7 +1131,7 @@
         <f aca="false">B11+$F$6</f>
         <v>576.070616100069</v>
       </c>
-      <c r="G11" s="4" t="n">
+      <c r="G11" s="5" t="n">
         <f aca="false">(F11/B11)*C11</f>
         <v>0.433198928035657</v>
       </c>
@@ -1136,7 +1159,7 @@
         <f aca="false">B12+$F$6</f>
         <v>581.806406655491</v>
       </c>
-      <c r="G12" s="4" t="n">
+      <c r="G12" s="5" t="n">
         <f aca="false">(F12/B12)*C12</f>
         <v>0.433148989271428</v>
       </c>
@@ -1164,7 +1187,7 @@
         <f aca="false">B13+$F$6</f>
         <v>587.542197210914</v>
       </c>
-      <c r="G13" s="4" t="n">
+      <c r="G13" s="5" t="n">
         <f aca="false">(F13/B13)*C13</f>
         <v>0.432634651944741</v>
       </c>
@@ -1192,7 +1215,7 @@
         <f aca="false">B14+$F$6</f>
         <v>593.277987766337</v>
       </c>
-      <c r="G14" s="4" t="n">
+      <c r="G14" s="5" t="n">
         <f aca="false">(F14/B14)*C14</f>
         <v>0.430575709615809</v>
       </c>
@@ -1220,7 +1243,7 @@
         <f aca="false">B15+$F$6</f>
         <v>599.013778321759</v>
       </c>
-      <c r="G15" s="4" t="n">
+      <c r="G15" s="5" t="n">
         <f aca="false">(F15/B15)*C15</f>
         <v>0.427940913154533</v>
       </c>
@@ -1248,7 +1271,7 @@
         <f aca="false">B16+$F$6</f>
         <v>604.749568877181</v>
       </c>
-      <c r="G16" s="4" t="n">
+      <c r="G16" s="5" t="n">
         <f aca="false">(F16/B16)*C16</f>
         <v>0.424133789472565</v>
       </c>
@@ -1276,7 +1299,7 @@
         <f aca="false">B17+$F$6</f>
         <v>610.485359432604</v>
       </c>
-      <c r="G17" s="4" t="n">
+      <c r="G17" s="5" t="n">
         <f aca="false">(F17/B17)*C17</f>
         <v>0.420356039356484</v>
       </c>
@@ -1304,19 +1327,19 @@
         <f aca="false">B18+$F$6</f>
         <v>616.221149988027</v>
       </c>
-      <c r="G18" s="4" t="n">
+      <c r="G18" s="5" t="n">
         <f aca="false">(F18/B18)*C18</f>
         <v>0.415412968261388</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>